<commit_message>
- Edit program list - Add custom program - add dcb2.0 database
</commit_message>
<xml_diff>
--- a/PE/pe_database.xlsx
+++ b/PE/pe_database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F31F733-623A-4ED6-A26F-05D6DB336263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DA03FF-3447-468C-9070-71645B97744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="7" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
   <sheets>
     <sheet name="bmw" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Contact Pairs</t>
   </si>
@@ -106,9 +106,6 @@
     <t>DCB1.2H</t>
   </si>
   <si>
-    <t>DCB2.0</t>
-  </si>
-  <si>
     <t>5DH</t>
   </si>
   <si>
@@ -116,17 +113,29 @@
   </si>
   <si>
     <t>CUSTOM</t>
+  </si>
+  <si>
+    <t>DCB_SH to MPEC</t>
+  </si>
+  <si>
+    <t>DCB_BC to MPEC</t>
+  </si>
+  <si>
+    <t>DCB_BC to MPE</t>
+  </si>
+  <si>
+    <t>DCB_SH to MPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -473,17 +482,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25B58C-B2FA-47E7-BFF1-8BC18104189A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -499,7 +508,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -507,7 +516,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -515,7 +524,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -536,13 +545,13 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -568,13 +577,13 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -590,7 +599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -598,7 +607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -606,7 +615,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -614,7 +623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -622,7 +631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -630,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -638,7 +647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -646,7 +655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -654,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -662,7 +671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -670,7 +679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -678,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -686,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -694,7 +703,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -702,7 +711,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -710,7 +719,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -718,7 +727,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -726,7 +735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -734,7 +743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -755,13 +764,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -781,19 +790,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECD227B-6E8F-43BD-BC3F-E2F60B91D590}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -801,9 +810,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -819,13 +855,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -833,9 +869,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -851,13 +887,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -865,9 +901,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -879,17 +915,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0778F-CE7F-4479-A4FA-B54BCE8E62E6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -897,9 +933,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Command DMM(port2) 600mS by use dangerTime when on DC-Source - Get data convert format EX.+2.37400000E-02 --> 23.740 mV - Identify DMM have value --> Use manual - Get set point from database to automatic set and send to comPort1 - Clean and Check every grammar and comment
</commit_message>
<xml_diff>
--- a/PE/pe_database.xlsx
+++ b/PE/pe_database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DA03FF-3447-468C-9070-71645B97744F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1BAA99-25AA-4C4F-8BF8-D351A49AA9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{F46F73B6-9C4F-47DE-B779-0A6401A94E00}"/>
   </bookViews>
   <sheets>
     <sheet name="bmw" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>Contact Pairs</t>
   </si>
@@ -106,6 +106,9 @@
     <t>DCB1.2H</t>
   </si>
   <si>
+    <t>DCB2.0</t>
+  </si>
+  <si>
     <t>5DH</t>
   </si>
   <si>
@@ -115,27 +118,21 @@
     <t>CUSTOM</t>
   </si>
   <si>
-    <t>DCB_SH to MPEC</t>
-  </si>
-  <si>
-    <t>DCB_BC to MPEC</t>
-  </si>
-  <si>
-    <t>DCB_BC to MPE</t>
-  </si>
-  <si>
-    <t>DCB_SH to MPE</t>
+    <t>Setpoint Voltage</t>
+  </si>
+  <si>
+    <t>Setpoint Current</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <charset val="222"/>
       <scheme val="minor"/>
@@ -480,35 +477,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C25B58C-B2FA-47E7-BFF1-8BC18104189A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -516,7 +526,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -524,7 +534,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -539,29 +549,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B3C947-D757-45AA-817A-4B43C428C667}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -571,35 +591,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E4A438-F966-48A2-AFD5-D9139D663046}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C1" sqref="C1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -607,7 +640,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -615,7 +648,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -623,7 +656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -631,7 +664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -639,7 +672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -647,7 +680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -655,7 +688,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -663,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -671,7 +704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -679,7 +712,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -687,7 +720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -695,7 +728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -703,7 +736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -711,7 +744,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -719,7 +752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -727,7 +760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -735,7 +768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
@@ -743,7 +776,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -758,27 +791,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C5E0E7-8060-4401-A9FF-74A0D7403DC3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -790,56 +830,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECD227B-6E8F-43BD-BC3F-E2F60B91D590}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C2" sqref="C2:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -849,29 +869,36 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603C8D41-01FC-4D0E-92B9-31FA79835127}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -881,29 +908,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A96459A-EFE5-49DC-B9F0-72C636BBE5E1}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -913,29 +947,36 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD0778F-CE7F-4479-A4FA-B54BCE8E62E6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>